<commit_message>
Further Edit to Board Codes in Table 3
</commit_message>
<xml_diff>
--- a/reference_files/Table3-Crude-Mortality-population-based-and-30-day-from-discharge.xlsx
+++ b/reference_files/Table3-Crude-Mortality-population-based-and-30-day-from-discharge.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
   <si>
     <t>Scotland</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t xml:space="preserve">Only Teaching, Large and Small General Hospitals are presented individually, whilst NHS Board figures will include all acute patients treated within the NHS Board area. </t>
+  </si>
+  <si>
+    <t>S08000031</t>
   </si>
 </sst>
 </file>
@@ -1051,7 +1054,6 @@
           </c:strCache>
         </c:strRef>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1513,7 +1515,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -21710,7 +21711,7 @@
   <dimension ref="A1:B51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21769,7 +21770,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="34" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B7" s="34" t="s">
         <v>17</v>

</xml_diff>